<commit_message>
Updated Bayesian calibration example
</commit_message>
<xml_diff>
--- a/Example/Parameter_UQ_Repository_V1.0.xlsx
+++ b/Example/Parameter_UQ_Repository_V1.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2FF88C-DB08-428F-86BE-A10BBF5DAD39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218E6BE-F0F7-4AD8-B42C-95E53D8211BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="1920" windowWidth="23040" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UQ" sheetId="1" r:id="rId1"/>
@@ -985,8 +985,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1898,7 +1898,7 @@
         <v>65</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="30" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Update default glazing uncertainty
</commit_message>
<xml_diff>
--- a/Example/Parameter_UQ_Repository_V1.0.xlsx
+++ b/Example/Parameter_UQ_Repository_V1.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218E6BE-F0F7-4AD8-B42C-95E53D8211BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47602859-E84B-447B-8D9F-2C6CAD3BE2B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UQ" sheetId="1" r:id="rId1"/>
@@ -985,8 +985,8 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1284,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H11" s="32">
         <v>0</v>
@@ -1311,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H12" s="32">
         <v>0</v>
@@ -1338,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H13" s="32">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H14" s="32">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H15" s="32">
         <v>0</v>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H16" s="32">
         <v>0</v>
@@ -1446,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H17" s="32">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H18" s="32">
         <v>0</v>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="6">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H19" s="32">
         <v>0</v>

</xml_diff>